<commit_message>
error correction of std
</commit_message>
<xml_diff>
--- a/result/results.xlsx
+++ b/result/results.xlsx
@@ -764,11 +764,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="237533168"/>
-        <c:axId val="237152408"/>
+        <c:axId val="1328336752"/>
+        <c:axId val="1328337296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="237533168"/>
+        <c:axId val="1328336752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -808,7 +808,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237152408"/>
+        <c:crossAx val="1328337296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -816,7 +816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237152408"/>
+        <c:axId val="1328337296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -865,7 +865,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237533168"/>
+        <c:crossAx val="1328336752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1297,11 +1297,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="238234136"/>
-        <c:axId val="238232960"/>
+        <c:axId val="1396859760"/>
+        <c:axId val="1396860304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="238234136"/>
+        <c:axId val="1396859760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,7 +1344,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238232960"/>
+        <c:crossAx val="1396860304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,7 +1352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238232960"/>
+        <c:axId val="1396860304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1464,7 +1464,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238234136"/>
+        <c:crossAx val="1396859760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1930,11 +1930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="236446976"/>
-        <c:axId val="236447368"/>
+        <c:axId val="1328336208"/>
+        <c:axId val="1328337840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="236446976"/>
+        <c:axId val="1328336208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2045,12 +2045,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236447368"/>
+        <c:crossAx val="1328337840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236447368"/>
+        <c:axId val="1328337840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2164,7 +2164,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236446976"/>
+        <c:crossAx val="1328336208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2641,8 +2641,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236445408"/>
-        <c:axId val="236444232"/>
+        <c:axId val="1328335120"/>
+        <c:axId val="1328340560"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2995,11 +2995,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236445800"/>
-        <c:axId val="236446192"/>
+        <c:axId val="1328342192"/>
+        <c:axId val="1328341104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236445408"/>
+        <c:axId val="1328335120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3042,7 +3042,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236444232"/>
+        <c:crossAx val="1328340560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3050,7 +3050,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236444232"/>
+        <c:axId val="1328340560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3163,12 +3163,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236445408"/>
+        <c:crossAx val="1328335120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="236446192"/>
+        <c:axId val="1328341104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3265,12 +3265,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236445800"/>
+        <c:crossAx val="1328342192"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="236445800"/>
+        <c:axId val="1328342192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3280,7 +3280,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236446192"/>
+        <c:crossAx val="1328341104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3799,8 +3799,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236444624"/>
-        <c:axId val="237420264"/>
+        <c:axId val="1326678608"/>
+        <c:axId val="1326682416"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4161,11 +4161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237417520"/>
-        <c:axId val="237419088"/>
+        <c:axId val="1326683504"/>
+        <c:axId val="1326681872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236444624"/>
+        <c:axId val="1326678608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4208,7 +4208,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237420264"/>
+        <c:crossAx val="1326682416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4216,7 +4216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237420264"/>
+        <c:axId val="1326682416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4329,12 +4329,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236444624"/>
+        <c:crossAx val="1326678608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237419088"/>
+        <c:axId val="1326681872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4431,12 +4431,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237417520"/>
+        <c:crossAx val="1326683504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="237417520"/>
+        <c:axId val="1326683504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4446,7 +4446,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237419088"/>
+        <c:crossAx val="1326681872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4965,8 +4965,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237415560"/>
-        <c:axId val="237419872"/>
+        <c:axId val="1326677520"/>
+        <c:axId val="1326679696"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5327,11 +5327,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237415952"/>
-        <c:axId val="237416344"/>
+        <c:axId val="1326679152"/>
+        <c:axId val="1326678064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237415560"/>
+        <c:axId val="1326677520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5374,7 +5374,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237419872"/>
+        <c:crossAx val="1326679696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5382,7 +5382,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237419872"/>
+        <c:axId val="1326679696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5495,12 +5495,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237415560"/>
+        <c:crossAx val="1326677520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237416344"/>
+        <c:axId val="1326678064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5597,12 +5597,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237415952"/>
+        <c:crossAx val="1326679152"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="237415952"/>
+        <c:axId val="1326679152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5612,7 +5612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237416344"/>
+        <c:crossAx val="1326678064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6127,8 +6127,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237421048"/>
-        <c:axId val="237416736"/>
+        <c:axId val="1326681328"/>
+        <c:axId val="1397409280"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6489,11 +6489,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237422224"/>
-        <c:axId val="237421440"/>
+        <c:axId val="1397411456"/>
+        <c:axId val="1397414176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237421048"/>
+        <c:axId val="1326681328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6536,7 +6536,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237416736"/>
+        <c:crossAx val="1397409280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6544,7 +6544,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237416736"/>
+        <c:axId val="1397409280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6655,12 +6655,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237421048"/>
+        <c:crossAx val="1326681328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237421440"/>
+        <c:axId val="1397414176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6757,12 +6757,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237422224"/>
+        <c:crossAx val="1397411456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="237422224"/>
+        <c:axId val="1397411456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6772,7 +6772,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237421440"/>
+        <c:crossAx val="1397414176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7210,11 +7210,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="237415168"/>
-        <c:axId val="238230608"/>
+        <c:axId val="1397412544"/>
+        <c:axId val="1397410368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="237415168"/>
+        <c:axId val="1397412544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7257,7 +7257,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238230608"/>
+        <c:crossAx val="1397410368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7265,7 +7265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238230608"/>
+        <c:axId val="1397410368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7377,7 +7377,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237415168"/>
+        <c:crossAx val="1397412544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7788,11 +7788,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="238231392"/>
-        <c:axId val="238232568"/>
+        <c:axId val="1397408736"/>
+        <c:axId val="1397407104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="238231392"/>
+        <c:axId val="1397408736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7835,7 +7835,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238232568"/>
+        <c:crossAx val="1397407104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7843,7 +7843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238232568"/>
+        <c:axId val="1397407104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7955,7 +7955,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238231392"/>
+        <c:crossAx val="1397408736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8366,11 +8366,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="238232176"/>
-        <c:axId val="238230216"/>
+        <c:axId val="1397408192"/>
+        <c:axId val="1396854320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="238232176"/>
+        <c:axId val="1397408192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8413,7 +8413,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238230216"/>
+        <c:crossAx val="1396854320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8421,7 +8421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238230216"/>
+        <c:axId val="1396854320"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8533,7 +8533,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238232176"/>
+        <c:crossAx val="1397408192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14716,8 +14716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:S62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>